<commit_message>
Invoice to Sale feature added
</commit_message>
<xml_diff>
--- a/extracted.xlsx
+++ b/extracted.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V7"/>
+  <dimension ref="A1:V21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -548,7 +548,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>panty</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -558,7 +558,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Badol paul</t>
+          <t>HashemAlom</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -568,7 +568,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>175251327743686272</t>
+          <t>175556396517968896</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -578,22 +578,22 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>175251327743686272</t>
+          <t>175556396517968896</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>wh1yp262031</t>
+          <t>wh1yp262035</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>11.07.2025</t>
+          <t>12.07.2025</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>11.07.2025</t>
+          <t>12.07.2025</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -648,19 +648,19 @@
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>Rs.8.62</t>
+          <t>Rs.9.62</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>West Bengal</t>
+          <t>Meghalaya</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>panty</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -670,7 +670,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Lokanathan G</t>
+          <t>SujalNikam</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -680,22 +680,22 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1490815352952096</t>
+          <t>1490815374383440</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Prepaid: Do not collect cash</t>
+          <t>COD</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>175327057083911168</t>
+          <t>175558215541476608</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>wh1yp262032</t>
+          <t>wh1yp262037</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -715,7 +715,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>90cm</t>
+          <t>85cm</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
@@ -760,19 +760,19 @@
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>Rs.8.33</t>
+          <t>Rs.9.00</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>Tamil Nadu</t>
+          <t>Maharashtra</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>panty</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -782,17 +782,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Rahul</t>
+          <t>Sonam Kumari</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Shadowfax</t>
+          <t>Valmo</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>175488445392877376</t>
+          <t>175561098886401152</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -802,12 +802,12 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>175488445392877376</t>
+          <t>175561098886401152</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>wh1yp262034</t>
+          <t>wh1yp262040</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -827,7 +827,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>90cm</t>
+          <t>85cm</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
@@ -872,29 +872,29 @@
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>Rs.8.95</t>
+          <t>Rs.8.91</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>Uttar Pradesh</t>
+          <t>Karnataka</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>panty</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>5</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Reena</t>
+          <t>Priyanka Naganur</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -904,32 +904,32 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>175432277122108608</t>
+          <t>175777324985481024</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>COD</t>
+          <t>Prepaid: Do not collect cash</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>175432277122108608</t>
+          <t>175777324985481024</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>wh1yp262033</t>
+          <t>wh1yp262049</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>12.07.2025</t>
+          <t>13.07.2025</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>12.07.2025</t>
+          <t>13.07.2025</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -939,7 +939,7 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>XS</t>
+          <t>85cm</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
@@ -989,14 +989,14 @@
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>Uttar Pradesh</t>
+          <t>Karnataka</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>panty</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1006,17 +1006,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Arhan Arman</t>
+          <t>yogesh ghumre</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Shadowfax</t>
+          <t>Valmo</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>175129190839452992</t>
+          <t>175557886137617344</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1026,22 +1026,22 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>175129190839452992</t>
+          <t>175557886137617344</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>wh1yp262018</t>
+          <t>wh1yp262036</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>11.07.2025</t>
+          <t>12.07.2025</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>11.07.2025</t>
+          <t>12.07.2025</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -1096,124 +1096,1692 @@
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>Rs.8.91</t>
+          <t>Rs.8.95</t>
         </is>
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>Karnataka</t>
+          <t>Maharashtra</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>panty</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>5</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Prashant</t>
+          <t>Nilima. Chatterjee</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
+          <t>Valmo</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>175602238777194176</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Prepaid: Do not collect cash</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>175602238777194176</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>wh1yp262047</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>12.07.2025</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>12.07.2025</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>HSN</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>90cm</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>Color</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>Rs.7.33</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>Jharkhand</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>camisole</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>md ahsan alam</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Valmo</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>175559048513473472</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>COD</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>175559048513473472</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>wh1yp262039</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>12.07.2025</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>12.07.2025</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>HSN</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>Color</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>Rs.7.52</t>
+        </is>
+      </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>Bihar</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>camisole</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Sana Parveen</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Valmo</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>175569396977126528</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>COD</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>175569396977126528</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>wh1yp262044</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>12.07.2025</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>12.07.2025</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>HSN</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>Color</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>Rs.6.71</t>
+        </is>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>Bihar</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>camisole</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Lopamudra Mohapatra</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Valmo</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>175582101089023872</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>COD</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>175582101089023872</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>wh1yp262045</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>12.07.2025</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>12.07.2025</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>HSN</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>Color</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>Rs.6.57</t>
+        </is>
+      </c>
+      <c r="V10" t="inlineStr">
+        <is>
+          <t>Odisha</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>camisole</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Fatima</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Valmo</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>175583658634136704</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>COD</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>175583658634136704</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>wh1yp262046</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>12.07.2025</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>12.07.2025</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>HSN</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>Color</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>Rs.6.95</t>
+        </is>
+      </c>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>Rajasthan</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>camisole</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>abhishekkumar</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Valmo</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>175785844262827648</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Prepaid: Do not collect cash</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>175785844262827648</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>wh1yp262050</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>13.07.2025</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>13.07.2025</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>HSN</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>Color</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>Rs.6.81</t>
+        </is>
+      </c>
+      <c r="V12" t="inlineStr">
+        <is>
+          <t>Uttar Pradesh</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>camisole</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>ansh kumar</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Shadowfax</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>175792758027712256</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>COD</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>175792758027712256</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>wh1yp262052</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>13.07.2025</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>13.07.2025</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>HSN</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>Color</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>Rs.6.71</t>
+        </is>
+      </c>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t>Bihar</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>camisole</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>PRIYANKA SETHIYA</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Valmo</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>175801950759286592</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Prepaid: Do not collect cash</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>175801950759286592</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>wh1yp262053</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>13.07.2025</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>13.07.2025</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>HSN</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>Color</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>Rs.6.10</t>
+        </is>
+      </c>
+      <c r="V14" t="inlineStr">
+        <is>
+          <t>Chhattisgarh</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>camisole</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>priti kushwaha</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Valmo</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>175805390238272576</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>COD</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>175805390238272576</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>wh1yp262054</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>13.07.2025</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>13.07.2025</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>HSN</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>Color</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>Rs.7.76</t>
+        </is>
+      </c>
+      <c r="V15" t="inlineStr">
+        <is>
+          <t>Madhya Pradesh</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>camisole</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>kathiravan</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Shadowfax</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>175558673123265728</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>COD</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>175558673123265728</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>wh1yp262038</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>12.07.2025</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>12.07.2025</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>HSN</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>Color</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>Rs.6.95</t>
+        </is>
+      </c>
+      <c r="V16" t="inlineStr">
+        <is>
+          <t>Tamil Nadu</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>camisole</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>asif khan</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Shadowfax</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>175566302205725696</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>COD</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>175566302205725696</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>wh1yp262041</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>12.07.2025</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>12.07.2025</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>HSN</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>Color</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>Rs.7.71</t>
+        </is>
+      </c>
+      <c r="V17" t="inlineStr">
+        <is>
+          <t>Uttar Pradesh</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>camisole</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>md       shabbir</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
           <t>Delhivery</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>1490815332957215</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>1490815374383451</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
         <is>
           <t>COD</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>174085951436981568</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>wh1yp261960</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>08.07.2025</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>08.07.2025</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>175566625197782912</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>wh1yp262042</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>12.07.2025</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>12.07.2025</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
         <is>
           <t>HSN</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>S</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
         <is>
           <t>Color</t>
         </is>
       </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="T7" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="U7" t="inlineStr">
-        <is>
-          <t>Rs.7.52</t>
-        </is>
-      </c>
-      <c r="V7" t="inlineStr">
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="T18" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>Rs.7.71</t>
+        </is>
+      </c>
+      <c r="V18" t="inlineStr">
         <is>
           <t>Telangana</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>camisole</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Ruplekha</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Valmo</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>175568367388740672</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>COD</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>175568367388740672</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>wh1yp262043</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>12.07.2025</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>12.07.2025</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>HSN</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>Color</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="T19" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>Rs.8.48</t>
+        </is>
+      </c>
+      <c r="V19" t="inlineStr">
+        <is>
+          <t>Assam</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>camisole</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Revathy</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Delhivery</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>1490815374383462</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>COD</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>175652059540900992</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>wh1yp262048</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>12.07.2025</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>12.07.2025</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>HSN</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>Color</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="T20" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>Rs.7.48</t>
+        </is>
+      </c>
+      <c r="V20" t="inlineStr">
+        <is>
+          <t>Kerala</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>camisole</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>kajal singh</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Delhivery</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>1490815374383495</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>COD</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>175786099799510272</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>wh1yp262051</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>13.07.2025</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>13.07.2025</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>HSN</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>Color</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="T21" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>Rs.6.57</t>
+        </is>
+      </c>
+      <c r="V21" t="inlineStr">
+        <is>
+          <t>Jharkhand</t>
         </is>
       </c>
     </row>

</xml_diff>